<commit_message>
31 October first commit
</commit_message>
<xml_diff>
--- a/SCTestData/TestData.xlsx
+++ b/SCTestData/TestData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Pasword</t>
   </si>
@@ -150,6 +150,24 @@
   </si>
   <si>
     <t>WorkGroup1540808725081</t>
+  </si>
+  <si>
+    <t>UserName1540891228096</t>
+  </si>
+  <si>
+    <t>WorkGroup1540891352847</t>
+  </si>
+  <si>
+    <t>UserName1540892116953</t>
+  </si>
+  <si>
+    <t>WorkGroup1540892265445</t>
+  </si>
+  <si>
+    <t>UserName1540893075711</t>
+  </si>
+  <si>
+    <t>WorkGroup1540893191201</t>
   </si>
 </sst>
 </file>
@@ -523,10 +541,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resource Flow 29 November
</commit_message>
<xml_diff>
--- a/SCTestData/TestData.xlsx
+++ b/SCTestData/TestData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Pasword</t>
   </si>
@@ -249,6 +249,18 @@
   </si>
   <si>
     <t>WorkGroup1541055822256</t>
+  </si>
+  <si>
+    <t>UserName1542879668278</t>
+  </si>
+  <si>
+    <t>WorkGroup1542879828578</t>
+  </si>
+  <si>
+    <t>UserName1542882306701</t>
+  </si>
+  <si>
+    <t>WorkGroup1542882450361</t>
   </si>
 </sst>
 </file>
@@ -622,10 +634,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>